<commit_message>
modificada el callulo de hpras de informes
</commit_message>
<xml_diff>
--- a/src/AppPartes.Web/wwwroot/Horas_484.xlsx
+++ b/src/AppPartes.Web/wwwroot/Horas_484.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>JAVIER SAN MARTIN MUTILVA</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Dia:29</t>
+  </si>
+  <si>
+    <t>Dia:30</t>
   </si>
   <si>
     <t>FERNANDO VIANA ECHEVERRIA</t>
@@ -408,10 +411,13 @@
       <c r="AD2" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="AE2" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1">
         <v>8</v>
@@ -499,11 +505,14 @@
       </c>
       <c r="AD3" s="1">
         <v>8</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>9.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1">
         <v>8</v>
@@ -591,11 +600,14 @@
       </c>
       <c r="AD4" s="1">
         <v>8</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>9.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1">
         <v>8</v>
@@ -690,7 +702,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1">
         <v>8</v>
@@ -785,7 +797,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1">
         <v>8</v>
@@ -880,7 +892,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1">
         <v>8</v>
@@ -967,12 +979,15 @@
         <v>8</v>
       </c>
       <c r="AD8" s="1">
+        <v>8</v>
+      </c>
+      <c r="AE8" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1">
         <v>7.5</v>
@@ -1067,7 +1082,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
         <v>5.25</v>
@@ -1162,7 +1177,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1">
         <v>8</v>
@@ -1257,7 +1272,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1">
         <v>8</v>
@@ -1352,7 +1367,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1">
         <v>8</v>
@@ -1428,19 +1443,121 @@
       </c>
       <c r="Z13" s="1">
         <v>8</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1">
         <v>8</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0</v>
+      </c>
+      <c r="W14" s="2">
+        <v>0</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1">
         <v>8</v>
@@ -1535,7 +1652,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1">
         <v>8</v>
@@ -1630,7 +1747,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1">
         <v>8</v>
@@ -1725,7 +1842,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1">
         <v>8</v>
@@ -1738,11 +1855,89 @@
       </c>
       <c r="E18" s="1">
         <v>8</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2">
+        <v>0</v>
+      </c>
+      <c r="U18" s="2">
+        <v>0</v>
+      </c>
+      <c r="V18" s="2">
+        <v>0</v>
+      </c>
+      <c r="W18" s="2">
+        <v>0</v>
+      </c>
+      <c r="X18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B19" s="1">
         <v>8</v>
@@ -1837,7 +2032,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1">
         <v>8</v>
@@ -1932,20 +2127,20 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="1">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
         <v>3.75</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>7.5</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>3</v>
       </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
       <c r="F21" s="2">
         <v>0</v>
       </c>
@@ -2000,105 +2195,129 @@
       <c r="W21" s="2">
         <v>0</v>
       </c>
-      <c r="X21" s="1">
+      <c r="X21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="1">
         <v>0.5</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="1">
+        <v>52</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
         <v>8.5</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>8.25</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>6.5</v>
       </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
       <c r="F22" s="2">
         <v>0</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
         <v>8.5</v>
       </c>
-      <c r="H22" s="1">
-        <v>8</v>
-      </c>
       <c r="I22" s="1">
-        <v>8.25</v>
+        <v>8</v>
       </c>
       <c r="J22" s="1">
         <v>8.25</v>
       </c>
       <c r="K22" s="1">
+        <v>8.25</v>
+      </c>
+      <c r="L22" s="1">
         <v>6.5</v>
       </c>
-      <c r="L22" s="2">
-        <v>0</v>
-      </c>
       <c r="M22" s="2">
         <v>0</v>
       </c>
-      <c r="N22" s="1">
+      <c r="N22" s="2">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
         <v>8.25</v>
       </c>
-      <c r="O22" s="1">
-        <v>8</v>
-      </c>
       <c r="P22" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="1">
         <v>8.25</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="R22" s="1">
         <v>8.5</v>
       </c>
-      <c r="R22" s="1">
+      <c r="S22" s="1">
         <v>6.5</v>
       </c>
-      <c r="S22" s="2">
-        <v>0</v>
-      </c>
       <c r="T22" s="2">
         <v>0</v>
       </c>
-      <c r="U22" s="1">
+      <c r="U22" s="2">
+        <v>0</v>
+      </c>
+      <c r="V22" s="1">
         <v>8.25</v>
       </c>
-      <c r="V22" s="1">
-        <v>8</v>
-      </c>
       <c r="W22" s="1">
+        <v>8</v>
+      </c>
+      <c r="X22" s="1">
         <v>8.5</v>
       </c>
-      <c r="X22" s="1">
+      <c r="Y22" s="1">
         <v>8.25</v>
       </c>
-      <c r="Y22" s="1">
+      <c r="Z22" s="1">
         <v>6.5</v>
       </c>
-      <c r="Z22" s="2">
-        <v>0</v>
-      </c>
       <c r="AA22" s="2">
         <v>0</v>
       </c>
-      <c r="AB22" s="1">
+      <c r="AB22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="1">
         <v>8.25</v>
       </c>
-      <c r="AC22" s="1">
-        <v>8</v>
-      </c>
       <c r="AD22" s="1">
+        <v>8</v>
+      </c>
+      <c r="AE22" s="1">
         <v>8.25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1">
         <v>8</v>
@@ -2193,7 +2412,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" s="3">
         <v>8</v>
@@ -2288,7 +2507,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1">
         <v>8</v>
@@ -2383,7 +2602,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1">
         <v>9</v>
@@ -2478,7 +2697,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B27" s="1">
         <v>2</v>
@@ -2565,12 +2784,15 @@
         <v>8</v>
       </c>
       <c r="AD27" s="1">
+        <v>8</v>
+      </c>
+      <c r="AE27" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1">
         <v>8</v>
@@ -2665,7 +2887,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1">
         <v>8</v>
@@ -2760,7 +2982,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B30" s="1">
         <v>8</v>
@@ -2855,7 +3077,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B31" s="1">
         <v>10</v>
@@ -2950,7 +3172,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1">
         <v>8</v>
@@ -3037,12 +3259,15 @@
         <v>8</v>
       </c>
       <c r="AD32" s="1">
+        <v>8</v>
+      </c>
+      <c r="AE32" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B33" s="1">
         <v>9</v>
@@ -3115,11 +3340,29 @@
       </c>
       <c r="Y33" s="1">
         <v>6</v>
+      </c>
+      <c r="Z33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1">
         <v>12</v>
@@ -3214,7 +3457,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1">
         <v>10</v>
@@ -3309,7 +3552,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" s="1">
         <v>10</v>
@@ -3404,36 +3647,123 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="1">
+        <v>67</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1">
         <v>1</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0</v>
+      </c>
+      <c r="M37" s="2">
+        <v>0</v>
+      </c>
+      <c r="N37" s="2">
+        <v>0</v>
+      </c>
+      <c r="O37" s="2">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>0</v>
+      </c>
+      <c r="R37" s="2">
+        <v>0</v>
+      </c>
+      <c r="S37" s="2">
+        <v>0</v>
+      </c>
+      <c r="T37" s="2">
+        <v>0</v>
+      </c>
+      <c r="U37" s="2">
+        <v>0</v>
+      </c>
+      <c r="V37" s="2">
+        <v>0</v>
+      </c>
+      <c r="W37" s="2">
+        <v>0</v>
+      </c>
+      <c r="X37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="1">
-        <v>8</v>
-      </c>
-      <c r="C38" s="1">
-        <v>8</v>
-      </c>
-      <c r="D38" s="1">
-        <v>8</v>
-      </c>
-      <c r="E38" s="1">
-        <v>8</v>
-      </c>
-      <c r="F38" s="1">
-        <v>8</v>
+        <v>68</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
       </c>
       <c r="G38" s="2">
         <v>0</v>
       </c>
-      <c r="H38" s="2">
-        <v>0</v>
+      <c r="H38" s="1">
+        <v>8</v>
       </c>
       <c r="I38" s="1">
         <v>8</v>
@@ -3447,46 +3777,67 @@
       <c r="L38" s="1">
         <v>8</v>
       </c>
-      <c r="M38" s="1">
-        <v>8</v>
+      <c r="M38" s="2">
+        <v>0</v>
       </c>
       <c r="N38" s="2">
         <v>0</v>
       </c>
-      <c r="O38" s="2">
-        <v>0</v>
+      <c r="O38" s="1">
+        <v>8</v>
       </c>
       <c r="P38" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>8</v>
+      </c>
+      <c r="R38" s="1">
+        <v>8</v>
+      </c>
+      <c r="S38" s="1">
+        <v>8</v>
+      </c>
+      <c r="T38" s="2">
+        <v>0</v>
+      </c>
+      <c r="U38" s="2">
+        <v>0</v>
+      </c>
+      <c r="V38" s="1">
         <v>10.5</v>
       </c>
-      <c r="Q38" s="1">
-        <v>8</v>
-      </c>
-      <c r="R38" s="1">
-        <v>8</v>
-      </c>
-      <c r="S38" s="1">
-        <v>8</v>
-      </c>
-      <c r="T38" s="1">
-        <v>8</v>
-      </c>
-      <c r="U38" s="2">
-        <v>0</v>
-      </c>
-      <c r="V38" s="2">
-        <v>0</v>
-      </c>
       <c r="W38" s="1">
         <v>8</v>
       </c>
       <c r="X38" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y38" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="1">
+        <v>8</v>
+      </c>
+      <c r="AD38" s="1">
+        <v>8</v>
+      </c>
+      <c r="AE38" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B39" s="1">
         <v>8</v>
@@ -3581,58 +3932,145 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="1">
+        <v>70</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2">
+        <v>0</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2">
+        <v>0</v>
+      </c>
+      <c r="O40" s="2">
+        <v>0</v>
+      </c>
+      <c r="P40" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>0</v>
+      </c>
+      <c r="R40" s="2">
+        <v>0</v>
+      </c>
+      <c r="S40" s="2">
+        <v>0</v>
+      </c>
+      <c r="T40" s="2">
+        <v>0</v>
+      </c>
+      <c r="U40" s="2">
+        <v>0</v>
+      </c>
+      <c r="V40" s="2">
+        <v>0</v>
+      </c>
+      <c r="W40" s="2">
+        <v>0</v>
+      </c>
+      <c r="X40" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="1">
         <v>4</v>
+      </c>
+      <c r="Z40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="3">
+        <v>71</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3">
         <v>2.5</v>
       </c>
-      <c r="C41" s="3">
+      <c r="D41" s="3">
         <v>1</v>
       </c>
-      <c r="D41" s="3">
+      <c r="E41" s="3">
         <v>2</v>
       </c>
-      <c r="E41" s="4">
+      <c r="F41" s="4">
         <v>1.5</v>
       </c>
-      <c r="F41" s="2">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1">
+      <c r="G41" s="2">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
         <v>1</v>
       </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
         <v>5</v>
       </c>
-      <c r="I41" s="1">
+      <c r="J41" s="1">
         <v>2</v>
       </c>
-      <c r="J41" s="1">
+      <c r="K41" s="1">
         <v>2.5</v>
       </c>
-      <c r="K41" s="1">
+      <c r="L41" s="1">
         <v>3</v>
       </c>
-      <c r="L41" s="1">
+      <c r="M41" s="1">
         <v>1.5</v>
       </c>
-      <c r="M41" s="2">
-        <v>0</v>
-      </c>
-      <c r="N41" s="1">
+      <c r="N41" s="2">
+        <v>0</v>
+      </c>
+      <c r="O41" s="1">
         <v>2</v>
       </c>
-      <c r="O41" s="2">
-        <v>0</v>
-      </c>
       <c r="P41" s="2">
         <v>0</v>
       </c>
@@ -3642,14 +4080,14 @@
       <c r="R41" s="2">
         <v>0</v>
       </c>
-      <c r="S41" s="1">
+      <c r="S41" s="2">
+        <v>0</v>
+      </c>
+      <c r="T41" s="1">
         <v>1.5</v>
       </c>
-      <c r="T41" s="2">
-        <v>0</v>
-      </c>
-      <c r="U41" s="1">
-        <v>2</v>
+      <c r="U41" s="2">
+        <v>0</v>
       </c>
       <c r="V41" s="1">
         <v>2</v>
@@ -3658,32 +4096,128 @@
         <v>2</v>
       </c>
       <c r="X41" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y41" s="1">
         <v>1</v>
       </c>
-      <c r="Y41" s="1">
+      <c r="Z41" s="1">
         <v>3</v>
       </c>
-      <c r="Z41" s="1">
+      <c r="AA41" s="1">
         <v>1</v>
       </c>
-      <c r="AA41" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB41" s="1">
+      <c r="AB41" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="1">
         <v>1</v>
+      </c>
+      <c r="AD41" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE41" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="1">
+        <v>72</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2">
+        <v>0</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0</v>
+      </c>
+      <c r="M42" s="2">
+        <v>0</v>
+      </c>
+      <c r="N42" s="2">
+        <v>0</v>
+      </c>
+      <c r="O42" s="2">
+        <v>0</v>
+      </c>
+      <c r="P42" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>0</v>
+      </c>
+      <c r="R42" s="2">
+        <v>0</v>
+      </c>
+      <c r="S42" s="2">
+        <v>0</v>
+      </c>
+      <c r="T42" s="2">
+        <v>0</v>
+      </c>
+      <c r="U42" s="2">
+        <v>0</v>
+      </c>
+      <c r="V42" s="2">
+        <v>0</v>
+      </c>
+      <c r="W42" s="2">
+        <v>0</v>
+      </c>
+      <c r="X42" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="1">
         <v>0.5</v>
+      </c>
+      <c r="AD42" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B43" s="1">
         <v>8</v>
@@ -3778,7 +4312,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B44" s="1">
         <v>8</v>

</xml_diff>